<commit_message>
add multiqc table, delete pa vs qp table, and update shotgun table
</commit_message>
<xml_diff>
--- a/HJA_scripts/08_reference_sequences_datasets/shotgun_samples_HJAndrews_Malaisetraps_20200108.xlsx
+++ b/HJA_scripts/08_reference_sequences_datasets/shotgun_samples_HJAndrews_Malaisetraps_20200108.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Luo_Mingjie_Oregon/HJA_scripts/8_reference_sequences_datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Negorashi2011/Dropbox/Working_docs/Luo_Mingjie_Oregon/HJA_analyses_Kelpie/HJA_scripts/08_reference_sequences_datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22BDB036-8FB8-D246-A027-98B32FFE7DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB8295F-8F81-AA44-933B-4F4C700F5443}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="shotgun_samples_HJA_Malaise_fq" sheetId="1" r:id="rId1"/>
     <sheet name="pivot" sheetId="18" r:id="rId2"/>
-    <sheet name="HOBO_032" sheetId="14" r:id="rId3"/>
-    <sheet name="HOBO_036" sheetId="15" r:id="rId4"/>
+    <sheet name="HOBO_036" sheetId="15" r:id="rId3"/>
+    <sheet name="HOBO_032" sheetId="14" r:id="rId4"/>
     <sheet name="HOBO_357" sheetId="20" r:id="rId5"/>
     <sheet name="146764" sheetId="21" r:id="rId6"/>
     <sheet name="neighbors" sheetId="3" r:id="rId7"/>
@@ -28,7 +28,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId8"/>
+    <pivotCache cacheId="58" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -10465,7 +10465,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B52CC22D-6117-924F-8A27-B0F068C7E4BE}" name="PivotTable5" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B52CC22D-6117-924F-8A27-B0F068C7E4BE}" name="PivotTable5" cacheId="58" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" showDrill="0" itemPrintTitles="1" createdVersion="6" indent="0" showHeaders="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="A3:F102" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0" defaultSubtotal="0"/>
@@ -11235,6 +11235,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{50CAFFC3-24CC-D84D-A0FB-282BCA10F2EE}" name="Table12" displayName="Table12" ref="A1:H9" totalsRowShown="0">
+  <autoFilter ref="A1:H9" xr:uid="{A0BCFB37-59E8-454A-8732-9E45414D8A7A}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{3F5AECB5-56DC-C74E-A7DF-C9870187B678}" name="index"/>
+    <tableColumn id="2" xr3:uid="{359AB6AE-3013-E94E-BD65-EDA8DA838F9B}" name="fastq_files"/>
+    <tableColumn id="3" xr3:uid="{E1256813-13E4-9D4E-8895-4AFBF20D7925}" name="sample"/>
+    <tableColumn id="4" xr3:uid="{26C9BBA7-12A6-624A-88FC-8061951B8D36}" name="site"/>
+    <tableColumn id="5" xr3:uid="{2B06B710-9DBB-5E45-B0D8-36859740892A}" name="trap"/>
+    <tableColumn id="6" xr3:uid="{C705AD30-494E-594E-B129-95F9190D0840}" name="period"/>
+    <tableColumn id="7" xr3:uid="{BE07EAF4-DC37-FA4C-8CFC-98D1E2773B74}" name="UTM_E"/>
+    <tableColumn id="8" xr3:uid="{0241C8F2-4518-1A44-82F1-9EBB89B718B5}" name="UTM_N"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6637568F-1F71-7F4A-8C3E-070B11501C63}" name="Table11" displayName="Table11" ref="A1:H9" totalsRowShown="0">
   <autoFilter ref="A1:H9" xr:uid="{9C27F6BE-3B5C-2A4D-B766-BB76004874CF}"/>
   <tableColumns count="8">
@@ -11246,23 +11263,6 @@
     <tableColumn id="6" xr3:uid="{8CF7998D-7E1F-F149-A7FA-65F1B10E1CA3}" name="period"/>
     <tableColumn id="7" xr3:uid="{43616042-3155-1941-B95C-A133DA7320B0}" name="UTM_E"/>
     <tableColumn id="8" xr3:uid="{FFB9CBF0-05FA-684A-852E-A6F9EFF88D6B}" name="UTM_N"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{50CAFFC3-24CC-D84D-A0FB-282BCA10F2EE}" name="Table12" displayName="Table12" ref="A1:H9" totalsRowShown="0">
-  <autoFilter ref="A1:H9" xr:uid="{A0BCFB37-59E8-454A-8732-9E45414D8A7A}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3F5AECB5-56DC-C74E-A7DF-C9870187B678}" name="index"/>
-    <tableColumn id="2" xr3:uid="{359AB6AE-3013-E94E-BD65-EDA8DA838F9B}" name="fastq_files"/>
-    <tableColumn id="3" xr3:uid="{E1256813-13E4-9D4E-8895-4AFBF20D7925}" name="sample"/>
-    <tableColumn id="4" xr3:uid="{26C9BBA7-12A6-624A-88FC-8061951B8D36}" name="site"/>
-    <tableColumn id="5" xr3:uid="{2B06B710-9DBB-5E45-B0D8-36859740892A}" name="trap"/>
-    <tableColumn id="6" xr3:uid="{C705AD30-494E-594E-B129-95F9190D0840}" name="period"/>
-    <tableColumn id="7" xr3:uid="{BE07EAF4-DC37-FA4C-8CFC-98D1E2773B74}" name="UTM_E"/>
-    <tableColumn id="8" xr3:uid="{0241C8F2-4518-1A44-82F1-9EBB89B718B5}" name="UTM_N"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -11608,8 +11608,8 @@
   <dimension ref="A1:O485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C133" sqref="C133"/>
+      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28727,8 +28727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5180F7DA-2E41-4646-B5DD-AC312AD93B68}">
   <dimension ref="A3:V102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28736,7 +28736,7 @@
     <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
     <col min="2" max="4" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" customWidth="1"/>
     <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -32720,6 +32720,263 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1188648-DA6F-DB41-967E-DAFB83013113}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>292</v>
+      </c>
+      <c r="B2" t="s">
+        <v>449</v>
+      </c>
+      <c r="C2" t="s">
+        <v>448</v>
+      </c>
+      <c r="D2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>566184</v>
+      </c>
+      <c r="H2">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>291</v>
+      </c>
+      <c r="B3" t="s">
+        <v>447</v>
+      </c>
+      <c r="C3" t="s">
+        <v>448</v>
+      </c>
+      <c r="D3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>566184</v>
+      </c>
+      <c r="H3">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>290</v>
+      </c>
+      <c r="B4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C4" t="s">
+        <v>445</v>
+      </c>
+      <c r="D4" t="s">
+        <v>442</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>566184</v>
+      </c>
+      <c r="H4">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>289</v>
+      </c>
+      <c r="B5" t="s">
+        <v>444</v>
+      </c>
+      <c r="C5" t="s">
+        <v>445</v>
+      </c>
+      <c r="D5" t="s">
+        <v>442</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>566184</v>
+      </c>
+      <c r="H5">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>288</v>
+      </c>
+      <c r="B6" t="s">
+        <v>443</v>
+      </c>
+      <c r="C6" t="s">
+        <v>441</v>
+      </c>
+      <c r="D6" t="s">
+        <v>442</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>566184</v>
+      </c>
+      <c r="H6">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>287</v>
+      </c>
+      <c r="B7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" t="s">
+        <v>441</v>
+      </c>
+      <c r="D7" t="s">
+        <v>442</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>566184</v>
+      </c>
+      <c r="H7">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>294</v>
+      </c>
+      <c r="B8" t="s">
+        <v>452</v>
+      </c>
+      <c r="C8" t="s">
+        <v>451</v>
+      </c>
+      <c r="D8" t="s">
+        <v>442</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>566184</v>
+      </c>
+      <c r="H8">
+        <v>4897312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>293</v>
+      </c>
+      <c r="B9" t="s">
+        <v>450</v>
+      </c>
+      <c r="C9" t="s">
+        <v>451</v>
+      </c>
+      <c r="D9" t="s">
+        <v>442</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>566184</v>
+      </c>
+      <c r="H9">
+        <v>4897312</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F68417B4-45F9-6945-B1FB-93A75F427311}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -32966,263 +33223,6 @@
       </c>
       <c r="H9">
         <v>4895774</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1188648-DA6F-DB41-967E-DAFB83013113}">
-  <dimension ref="A1:H9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="49.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>775</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>292</v>
-      </c>
-      <c r="B2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C2" t="s">
-        <v>448</v>
-      </c>
-      <c r="D2" t="s">
-        <v>442</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>566184</v>
-      </c>
-      <c r="H2">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>291</v>
-      </c>
-      <c r="B3" t="s">
-        <v>447</v>
-      </c>
-      <c r="C3" t="s">
-        <v>448</v>
-      </c>
-      <c r="D3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>566184</v>
-      </c>
-      <c r="H3">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>290</v>
-      </c>
-      <c r="B4" t="s">
-        <v>446</v>
-      </c>
-      <c r="C4" t="s">
-        <v>445</v>
-      </c>
-      <c r="D4" t="s">
-        <v>442</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="G4">
-        <v>566184</v>
-      </c>
-      <c r="H4">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>289</v>
-      </c>
-      <c r="B5" t="s">
-        <v>444</v>
-      </c>
-      <c r="C5" t="s">
-        <v>445</v>
-      </c>
-      <c r="D5" t="s">
-        <v>442</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>2</v>
-      </c>
-      <c r="G5">
-        <v>566184</v>
-      </c>
-      <c r="H5">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>288</v>
-      </c>
-      <c r="B6" t="s">
-        <v>443</v>
-      </c>
-      <c r="C6" t="s">
-        <v>441</v>
-      </c>
-      <c r="D6" t="s">
-        <v>442</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6">
-        <v>566184</v>
-      </c>
-      <c r="H6">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>287</v>
-      </c>
-      <c r="B7" t="s">
-        <v>440</v>
-      </c>
-      <c r="C7" t="s">
-        <v>441</v>
-      </c>
-      <c r="D7" t="s">
-        <v>442</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>2</v>
-      </c>
-      <c r="G7">
-        <v>566184</v>
-      </c>
-      <c r="H7">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>294</v>
-      </c>
-      <c r="B8" t="s">
-        <v>452</v>
-      </c>
-      <c r="C8" t="s">
-        <v>451</v>
-      </c>
-      <c r="D8" t="s">
-        <v>442</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8">
-        <v>2</v>
-      </c>
-      <c r="G8">
-        <v>566184</v>
-      </c>
-      <c r="H8">
-        <v>4897312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>293</v>
-      </c>
-      <c r="B9" t="s">
-        <v>450</v>
-      </c>
-      <c r="C9" t="s">
-        <v>451</v>
-      </c>
-      <c r="D9" t="s">
-        <v>442</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>2</v>
-      </c>
-      <c r="G9">
-        <v>566184</v>
-      </c>
-      <c r="H9">
-        <v>4897312</v>
       </c>
     </row>
   </sheetData>
@@ -33778,8 +33778,8 @@
   <dimension ref="A1:D481"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A211" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>